<commit_message>
anh tuan ninh binh
</commit_message>
<xml_diff>
--- a/5. WS/1. Bộ phận bảo hành/1. Thực hiện sửa chữa bảo hành/nam2022/Thang12/1.NhanBH/NBH221212_LapDat.xlsx
+++ b/5. WS/1. Bộ phận bảo hành/1. Thực hiện sửa chữa bảo hành/nam2022/Thang12/1.NhanBH/NBH221212_LapDat.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
   <si>
     <t xml:space="preserve">STT </t>
   </si>
@@ -85,6 +85,9 @@
   </si>
   <si>
     <t>28-B3-E9-F5-0C-00-00-22</t>
+  </si>
+  <si>
+    <t>Nguyễn Minh Tùng</t>
   </si>
 </sst>
 </file>
@@ -502,6 +505,33 @@
     <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
@@ -540,33 +570,6 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -924,7 +927,7 @@
   <dimension ref="A1:I34"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+      <selection activeCell="D19" sqref="D19:F19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.25"/>
@@ -941,92 +944,92 @@
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="4"/>
       <c r="B1" s="5"/>
-      <c r="C1" s="49" t="s">
+      <c r="C1" s="36" t="s">
         <v>4</v>
       </c>
-      <c r="D1" s="49"/>
-      <c r="E1" s="49"/>
-      <c r="F1" s="50"/>
+      <c r="D1" s="36"/>
+      <c r="E1" s="36"/>
+      <c r="F1" s="37"/>
     </row>
     <row r="2" spans="1:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="6"/>
       <c r="B2" s="7"/>
-      <c r="C2" s="51" t="s">
+      <c r="C2" s="38" t="s">
         <v>15</v>
       </c>
-      <c r="D2" s="51"/>
-      <c r="E2" s="51"/>
-      <c r="F2" s="52"/>
+      <c r="D2" s="38"/>
+      <c r="E2" s="38"/>
+      <c r="F2" s="39"/>
     </row>
     <row r="3" spans="1:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="6"/>
       <c r="B3" s="7"/>
-      <c r="C3" s="51" t="s">
+      <c r="C3" s="38" t="s">
         <v>13</v>
       </c>
-      <c r="D3" s="51"/>
-      <c r="E3" s="51"/>
-      <c r="F3" s="52"/>
+      <c r="D3" s="38"/>
+      <c r="E3" s="38"/>
+      <c r="F3" s="39"/>
     </row>
     <row r="4" spans="1:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="8"/>
       <c r="B4" s="9"/>
-      <c r="C4" s="53" t="s">
+      <c r="C4" s="40" t="s">
         <v>9</v>
       </c>
-      <c r="D4" s="53"/>
-      <c r="E4" s="53"/>
-      <c r="F4" s="54"/>
+      <c r="D4" s="40"/>
+      <c r="E4" s="40"/>
+      <c r="F4" s="41"/>
     </row>
     <row r="5" spans="1:6" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="46" t="s">
+      <c r="A5" s="33" t="s">
         <v>5</v>
       </c>
-      <c r="B5" s="47"/>
-      <c r="C5" s="47"/>
-      <c r="D5" s="47"/>
-      <c r="E5" s="47"/>
-      <c r="F5" s="48"/>
+      <c r="B5" s="34"/>
+      <c r="C5" s="34"/>
+      <c r="D5" s="34"/>
+      <c r="E5" s="34"/>
+      <c r="F5" s="35"/>
     </row>
     <row r="6" spans="1:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="13"/>
-      <c r="B6" s="33" t="s">
+      <c r="B6" s="42" t="s">
         <v>18</v>
       </c>
-      <c r="C6" s="33"/>
-      <c r="D6" s="33"/>
-      <c r="E6" s="33"/>
-      <c r="F6" s="34"/>
+      <c r="C6" s="42"/>
+      <c r="D6" s="42"/>
+      <c r="E6" s="42"/>
+      <c r="F6" s="43"/>
     </row>
     <row r="7" spans="1:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="10"/>
-      <c r="B7" s="39" t="s">
+      <c r="B7" s="48" t="s">
         <v>6</v>
       </c>
-      <c r="C7" s="39"/>
-      <c r="D7" s="39"/>
-      <c r="E7" s="39"/>
-      <c r="F7" s="40"/>
+      <c r="C7" s="48"/>
+      <c r="D7" s="48"/>
+      <c r="E7" s="48"/>
+      <c r="F7" s="49"/>
     </row>
     <row r="8" spans="1:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="11"/>
-      <c r="B8" s="42" t="s">
+      <c r="B8" s="51" t="s">
         <v>14</v>
       </c>
-      <c r="C8" s="42"/>
-      <c r="D8" s="42"/>
-      <c r="E8" s="42"/>
-      <c r="F8" s="43"/>
+      <c r="C8" s="51"/>
+      <c r="D8" s="51"/>
+      <c r="E8" s="51"/>
+      <c r="F8" s="52"/>
     </row>
     <row r="9" spans="1:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="12"/>
-      <c r="B9" s="44" t="s">
+      <c r="B9" s="53" t="s">
         <v>12</v>
       </c>
-      <c r="C9" s="44"/>
-      <c r="D9" s="44"/>
-      <c r="E9" s="44"/>
-      <c r="F9" s="45"/>
+      <c r="C9" s="53"/>
+      <c r="D9" s="53"/>
+      <c r="E9" s="53"/>
+      <c r="F9" s="54"/>
     </row>
     <row r="10" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="16" t="s">
@@ -1076,23 +1079,23 @@
       <c r="A13" s="18"/>
       <c r="B13" s="19"/>
       <c r="C13" s="19"/>
-      <c r="D13" s="37" t="s">
+      <c r="D13" s="46" t="s">
         <v>20</v>
       </c>
-      <c r="E13" s="37"/>
-      <c r="F13" s="38"/>
+      <c r="E13" s="46"/>
+      <c r="F13" s="47"/>
     </row>
     <row r="14" spans="1:6" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="20"/>
-      <c r="B14" s="36" t="s">
+      <c r="B14" s="45" t="s">
         <v>8</v>
       </c>
-      <c r="C14" s="36"/>
-      <c r="D14" s="36" t="s">
+      <c r="C14" s="45"/>
+      <c r="D14" s="45" t="s">
         <v>3</v>
       </c>
-      <c r="E14" s="36"/>
-      <c r="F14" s="41"/>
+      <c r="E14" s="45"/>
+      <c r="F14" s="50"/>
     </row>
     <row r="15" spans="1:6" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="20"/>
@@ -1128,16 +1131,16 @@
       <c r="G18" s="2"/>
     </row>
     <row r="19" spans="1:7" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="35" t="s">
+      <c r="A19" s="44" t="s">
         <v>10</v>
       </c>
-      <c r="B19" s="35"/>
-      <c r="C19" s="35"/>
-      <c r="D19" s="35" t="s">
-        <v>10</v>
-      </c>
-      <c r="E19" s="35"/>
-      <c r="F19" s="35"/>
+      <c r="B19" s="44"/>
+      <c r="C19" s="44"/>
+      <c r="D19" s="44" t="s">
+        <v>22</v>
+      </c>
+      <c r="E19" s="44"/>
+      <c r="F19" s="44"/>
     </row>
     <row r="20" spans="1:7" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="24"/>
@@ -1165,11 +1168,6 @@
     </row>
   </sheetData>
   <mergeCells count="14">
-    <mergeCell ref="A5:F5"/>
-    <mergeCell ref="C1:F1"/>
-    <mergeCell ref="C2:F2"/>
-    <mergeCell ref="C3:F3"/>
-    <mergeCell ref="C4:F4"/>
     <mergeCell ref="B6:F6"/>
     <mergeCell ref="A19:C19"/>
     <mergeCell ref="B14:C14"/>
@@ -1179,6 +1177,11 @@
     <mergeCell ref="D19:F19"/>
     <mergeCell ref="B8:F8"/>
     <mergeCell ref="B9:F9"/>
+    <mergeCell ref="A5:F5"/>
+    <mergeCell ref="C1:F1"/>
+    <mergeCell ref="C2:F2"/>
+    <mergeCell ref="C3:F3"/>
+    <mergeCell ref="C4:F4"/>
   </mergeCells>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>